<commit_message>
complicating my data and my life, Player edition
</commit_message>
<xml_diff>
--- a/Data/DataImports.xlsx
+++ b/Data/DataImports.xlsx
@@ -9,12 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Book" sheetId="3" r:id="rId1"/>
     <sheet name="Chapter" sheetId="1" r:id="rId2"/>
     <sheet name="ChapterIcon" sheetId="2" r:id="rId3"/>
+    <sheet name="Player" sheetId="4" r:id="rId4"/>
+    <sheet name="PlayerAlias" sheetId="11" r:id="rId5"/>
+    <sheet name="Organization" sheetId="5" r:id="rId6"/>
+    <sheet name="Prophecy" sheetId="6" r:id="rId7"/>
+    <sheet name="ProphecyType" sheetId="7" r:id="rId8"/>
+    <sheet name="Country" sheetId="8" r:id="rId9"/>
+    <sheet name="Location" sheetId="9" r:id="rId10"/>
+    <sheet name="Episode" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="400">
   <si>
     <t>BookTitle</t>
   </si>
@@ -725,6 +733,507 @@
   </si>
   <si>
     <t>Winter's Heart</t>
+  </si>
+  <si>
+    <t>PlayerName</t>
+  </si>
+  <si>
+    <t>PlayerDetailDescription</t>
+  </si>
+  <si>
+    <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>OrganizationDetailDescription</t>
+  </si>
+  <si>
+    <t>ProphecyTypeName</t>
+  </si>
+  <si>
+    <t>ProphecyDescription</t>
+  </si>
+  <si>
+    <t>CountryName</t>
+  </si>
+  <si>
+    <t>LocationName</t>
+  </si>
+  <si>
+    <t>EpisodeName</t>
+  </si>
+  <si>
+    <t>EpisodeChapterDescription</t>
+  </si>
+  <si>
+    <t>PropheciesList</t>
+  </si>
+  <si>
+    <t>OrganizationsList</t>
+  </si>
+  <si>
+    <t>PlayersList</t>
+  </si>
+  <si>
+    <t>PlayerAliasName</t>
+  </si>
+  <si>
+    <t>Lews Therin Telamon</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Lord of the Morning</t>
+  </si>
+  <si>
+    <t>Elan Morin Tedronai</t>
+  </si>
+  <si>
+    <t>Ishamael</t>
+  </si>
+  <si>
+    <t>Betrayer of Hope</t>
+  </si>
+  <si>
+    <t>the Hundred Companions</t>
+  </si>
+  <si>
+    <t>OrganizationMemberList?</t>
+  </si>
+  <si>
+    <t>Ilyena Therin Moerelle</t>
+  </si>
+  <si>
+    <t>Ilyena Sunhair</t>
+  </si>
+  <si>
+    <t>Ilyena Moerelle Dalisar</t>
+  </si>
+  <si>
+    <t>the Dark One</t>
+  </si>
+  <si>
+    <t>Shai'tan</t>
+  </si>
+  <si>
+    <t>Great Lord of the Dark</t>
+  </si>
+  <si>
+    <t>Great Lord</t>
+  </si>
+  <si>
+    <t>Father of Lies</t>
+  </si>
+  <si>
+    <t>Sightblinder</t>
+  </si>
+  <si>
+    <t>Lord of the Grave</t>
+  </si>
+  <si>
+    <t>Shepherd of the Night</t>
+  </si>
+  <si>
+    <t>Heartsbane</t>
+  </si>
+  <si>
+    <t>Grassburner</t>
+  </si>
+  <si>
+    <t>Leafblighter</t>
+  </si>
+  <si>
+    <t>Lighteater</t>
+  </si>
+  <si>
+    <t>the Dark Lord</t>
+  </si>
+  <si>
+    <t>Soulblinder</t>
+  </si>
+  <si>
+    <t>Father of Storms</t>
+  </si>
+  <si>
+    <t>Lord of the Evening</t>
+  </si>
+  <si>
+    <t>Old Hob</t>
+  </si>
+  <si>
+    <t>Old Grim</t>
+  </si>
+  <si>
+    <t>Lord of the Twilight</t>
+  </si>
+  <si>
+    <t>Heartfang</t>
+  </si>
+  <si>
+    <t>Soulsbane</t>
+  </si>
+  <si>
+    <t>Caisen Hob</t>
+  </si>
+  <si>
+    <t>Bringer of Gales</t>
+  </si>
+  <si>
+    <t>Rand al'Thor</t>
+  </si>
+  <si>
+    <t>Bela</t>
+  </si>
+  <si>
+    <t>Tam al'Thor</t>
+  </si>
+  <si>
+    <t>Cenn Buie</t>
+  </si>
+  <si>
+    <t>Wit Congar</t>
+  </si>
+  <si>
+    <t>Bran al'Vere</t>
+  </si>
+  <si>
+    <t>Nynaeve al'Meara</t>
+  </si>
+  <si>
+    <t>Daise Congar</t>
+  </si>
+  <si>
+    <t>Mat Cauthon</t>
+  </si>
+  <si>
+    <t>Egwene al'Vere</t>
+  </si>
+  <si>
+    <t>Mistress al'Donel</t>
+  </si>
+  <si>
+    <t>Dav Ayellin</t>
+  </si>
+  <si>
+    <t>Elam Dowtry</t>
+  </si>
+  <si>
+    <t>Andor</t>
+  </si>
+  <si>
+    <t>Emond's Field</t>
+  </si>
+  <si>
+    <t>Mountains of Mist</t>
+  </si>
+  <si>
+    <t>Sand Hills</t>
+  </si>
+  <si>
+    <t>Westwood</t>
+  </si>
+  <si>
+    <t>The Two Rivers</t>
+  </si>
+  <si>
+    <t>Baerlon</t>
+  </si>
+  <si>
+    <t>Killed everyone of his relatives in his madness.  Called Dragon and Lord of the Morning. Once stood first among the Servants, and wore the Ring of Tamyrlin.  Sat on the High Seat, summoned the Nine Rods of Dominion, and led the Hundred Companions.  Humbled Elan Morin in the Hall of Servants, and defeated him at the gates of Paaran Disen.  When he regains some of his sanity, he kills himself with an enourmous amount of the One Power, creating the mountain Dragonmount.</t>
+  </si>
+  <si>
+    <t>Clothed in black.  Identifies himself as Elan Morin Tedronai, called Betrayer of Hope by Lews Therin.  Appears out of thin air, says he is there to take Lews Therin.  Heals Lews Therin so that he may remember killing his family.  Says that the Great Lord can bring back Ilyena.</t>
+  </si>
+  <si>
+    <t>An Emond's Field man, married to Daise Congar.  Stops Tam and Rand on their way into Emond's Field to complain.</t>
+  </si>
+  <si>
+    <t>Wisom of Emond's Field.  Wit Congar complains about her, until his wife Daise admonishes him to stay out of Women's Circle business.</t>
+  </si>
+  <si>
+    <t>Lives on a farm in the Westwood.  Son of Tam al'Thor.  Is unusually tall and fair, with light hair and eyes.  Mother was an outlander.  Close to being betrothed to Egwene al'Vere.  Friends with Matt Cauthon.  Tam and Rand enter Emond's Field. Along the way, Rand sees a black-cloaked horseman. Rand and Mat talk about the dark horseman.  Mat has also seen him.</t>
+  </si>
+  <si>
+    <t>An Emond's Field woman.  Complains to Bran al'Vere that the storks have not returned to Emond's Field.</t>
+  </si>
+  <si>
+    <t>Wife of Wit Congar.  Admonishes her husband to not interfere with Women's Circle business.</t>
+  </si>
+  <si>
+    <t>Son of Abell Cauthon.  Friends with Rand al'Thor.  Known as the town's prankster.  Talks with Rand about the black-cloaked rider.  Both boys have seen him.</t>
+  </si>
+  <si>
+    <t>Catches a badger with Mat Cauthon, plans to release it on the village green.  Mat told him about he black-cloaked man but he had not seen him.</t>
+  </si>
+  <si>
+    <t>Mat Cauthon told him about he black-cloaked man but he had not seen him.</t>
+  </si>
+  <si>
+    <t>Thatcher from Emond's field. Sits on the Village Council. Talks with Tam al'Thor and Bran al'Vere outside the Winespring Inn.</t>
+  </si>
+  <si>
+    <t>Shaggy brown mare belonging to Tam and Rand al'Thor.  Tam and Rand take her to Emonds Field.</t>
+  </si>
+  <si>
+    <t>Bran al'Vere's daughter.</t>
+  </si>
+  <si>
+    <t>Ba'alzamon</t>
+  </si>
+  <si>
+    <t>Harral Luhhan</t>
+  </si>
+  <si>
+    <t>Leads a meeting of the Village Council.</t>
+  </si>
+  <si>
+    <t>Meets with other members of the Village Council.</t>
+  </si>
+  <si>
+    <t>Rowan Hurn</t>
+  </si>
+  <si>
+    <t>An Emond's Field man and a member of the Village Council.  Attends Council meeting at the Winespring Inn.</t>
+  </si>
+  <si>
+    <t>Samel Crawe</t>
+  </si>
+  <si>
+    <t>An Emond's Field man.  Horse-faced with a long nose.  Member of the Village Council.  Meets with the Council in the Winespring Inn.</t>
+  </si>
+  <si>
+    <t>Meets with the Council.</t>
+  </si>
+  <si>
+    <t>Mayor of Emond's Field and owner of the Winespring Inn.  Father of Egwene al'Vere.    Speaks with Tam al'Thor and Cenn Buie about the odd weather.</t>
+  </si>
+  <si>
+    <t>Bran Al'Vere</t>
+  </si>
+  <si>
+    <t>Brandelwyn al'Vere</t>
+  </si>
+  <si>
+    <t>Jon Thane</t>
+  </si>
+  <si>
+    <t>Emond's Field miller.  Mill lies east of the Winespring Water.  Menber of the Village Council.  Meets with the council.</t>
+  </si>
+  <si>
+    <t>Marin al'Vere</t>
+  </si>
+  <si>
+    <t>Wife of Bran al'Vere.  Mother to Egwene al'Vere.</t>
+  </si>
+  <si>
+    <t>Adan al'Caar</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy.  Matt plays a trick on him, Ewin Finngar and Dag Coplin.</t>
+  </si>
+  <si>
+    <t>Ewin Finngar</t>
+  </si>
+  <si>
+    <t>Dag Coplin</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy. Tells Mat Cauthon and Rand al'Thor about Moiraine and Lan.  Later, meets Moiraine and she hands him a coin.</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy.   Mat plays a trick on him, Adan al'Caar and Ewin Finngar.</t>
+  </si>
+  <si>
+    <t>Alsbet Luhhan</t>
+  </si>
+  <si>
+    <t>Emond's Field blacksmith.  Husband to Alsbet Luhhan.  Perrin Aybara is his apprentice.  Member of Village Council.  Attends Council meeting at the Winespring Inn.</t>
+  </si>
+  <si>
+    <t>Emond's Field woman.  Wife of Harral Luhhan.  Furious because Mat Cauthon floured her dogs as a prank.</t>
+  </si>
+  <si>
+    <t>Covered Haral Luhhan's dogs in flour as a prank to scare Adan al'Caar, Ewin Finngar and Dag Coplin.  Meets Moiraine, who gives him a coin, and Lan.</t>
+  </si>
+  <si>
+    <t>Moiraine</t>
+  </si>
+  <si>
+    <t>Lan</t>
+  </si>
+  <si>
+    <t>Moiraine Damodred</t>
+  </si>
+  <si>
+    <t>al'Lan Mandragoran</t>
+  </si>
+  <si>
+    <t>Dai Shan</t>
+  </si>
+  <si>
+    <t>Aan'allein</t>
+  </si>
+  <si>
+    <t>Lews Therin</t>
+  </si>
+  <si>
+    <t>Elan Morin</t>
+  </si>
+  <si>
+    <t>Hu</t>
+  </si>
+  <si>
+    <t>Tad</t>
+  </si>
+  <si>
+    <t>A Stranger from outside the Two Rivers.  She gives coins to Rand al'Thor, Mat Cauthon, and Ewin Finngar.  Ewin received a silver penny, while the others receive a fat coin that bears a woman balancing a flame in her hand.</t>
+  </si>
+  <si>
+    <t>Ewin Finngar said that Nynaeve doesn't like Moiraine because she called her "child".</t>
+  </si>
+  <si>
+    <t>An Emond's Field man. He and his brother Tad are the stablemen at the Winespring Inn.  They take care of Bela and the wagon.</t>
+  </si>
+  <si>
+    <t>An Emond's Field man. He and his brother Hu are the stablemen at the Winespring Inn.  They take care of Bela and the wagon.</t>
+  </si>
+  <si>
+    <t>A stranger who arrvies with Moiraine.  Wears a color-shifting cloak. Follows Moiraine. Ewin Finngar thinks he is a Warder.</t>
+  </si>
+  <si>
+    <t>Padan Fain</t>
+  </si>
+  <si>
+    <t>Perrin Aybara</t>
+  </si>
+  <si>
+    <t>Bili Congar</t>
+  </si>
+  <si>
+    <t>Thom Merrilin</t>
+  </si>
+  <si>
+    <t>Emond's Field boy.  lacksmith apprenticed to Harral Luhhan.  Friends with Rand al'Thor and Mat Cauthon.  Saw the black-cloaked rider.  Given a fat coin by Moiraine.</t>
+  </si>
+  <si>
+    <t>An Emond's Field man who enjoys his drink.  Once named the Dark One and had very bad luck.</t>
+  </si>
+  <si>
+    <t>She has been training Egwene Al'Vere to be a Wisdom.  She approaches Rand, Mat and Perrin while they are talking about the Dragon.</t>
+  </si>
+  <si>
+    <t>Arrives with Nynave al'Meara.  Talks with Rand al'Thor alone, then walks away in a huff.  Mat Cauthon and Perrin Aybara tell her about the black-cloaked rider they saw.</t>
+  </si>
+  <si>
+    <t>Talks about the Dragon, Aes Sedai and the Dark One with Perrin and Rand.  They tell Egwene Al'Vere about the black-cloaked rider they saw.</t>
+  </si>
+  <si>
+    <t>Recalls that Padain Fain first took notice of the, Perrin and Mat the year before.  Talks about the Dragon, Aes Sedai and the Dark One with Perrin and Mat.  They tell Egwene Al'Vere about the black-cloaked rider they saw.</t>
+  </si>
+  <si>
+    <t>A Peddler who arrives in Emond's Field.  Tells about a false Dragon in Ghealdan.  He comes to Emonds Field every year.</t>
+  </si>
+  <si>
+    <t>Wife of Lews Therin.  Killed by Lews Therin.</t>
+  </si>
+  <si>
+    <t>Ewal Coplin</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy.  Rand al'Thor recalls punching Ewal for teasing him about his gray eyes.</t>
+  </si>
+  <si>
+    <t>A gleeman hired by the Village Council for the Bel Tine festival.  Was once a Courd bard.  Knows Padan Fain and does not like him.  Speaks briefly to the Rand, Perrin, Mat and to Moiraine.</t>
+  </si>
+  <si>
+    <t>Urges Bran al'Vere to invite Padan Fain in to the inn to talk to the Village Council.</t>
+  </si>
+  <si>
+    <t>Rand al'Thor's father.  Member of the Village Council.  The best archer in Emond's Field.  Tam and Rand walk to Emond's Field with Bela pulling a cart. He talks with the other townsfolk.</t>
+  </si>
+  <si>
+    <t>He, Rand and Perrin meet Thom Merrilin, who offers to tell stories. Mat expresses an interest in battles.</t>
+  </si>
+  <si>
+    <t>He, Rand and Mat meet Thom Merrilin, who offers to tell stories.</t>
+  </si>
+  <si>
+    <t>She and Lan talk briefly with Thom Merrilin.</t>
+  </si>
+  <si>
+    <t>He and Moiraine talk briefly with Thom Merrilin.</t>
+  </si>
+  <si>
+    <t>She argues with Bran al'Vere and Cenn Buie after the Council meeting.</t>
+  </si>
+  <si>
+    <t>Lem Thane</t>
+  </si>
+  <si>
+    <t>Bandry Crawe</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy, Jon Thane's son.  Also saw the black-cloaked rider.</t>
+  </si>
+  <si>
+    <t>An Emond's Field boy, son of Samel Crawe.  Also saw the black-cloaked rider.</t>
+  </si>
+  <si>
+    <t>Tells the boys that the Aes Sedai in Ghealdan will not pass through the Two Rivers.  He and Rand head back to their farm.</t>
+  </si>
+  <si>
+    <t>Narg</t>
+  </si>
+  <si>
+    <t>Oren Dautry</t>
+  </si>
+  <si>
+    <t>A farmer in the Westwood.  Closest neighbor to the al'Thor farm.</t>
+  </si>
+  <si>
+    <t>He gives Rand his sword. Trollocs attack the farm and he is wounded.</t>
+  </si>
+  <si>
+    <t>She, Rand, Mat and Perrin listen to Thom Merrilin.  She follows Nynaeve when she leaves the Council meeting.</t>
+  </si>
+  <si>
+    <t>A Trolloc.  Part of the party that attacks the al'Thor farm on Winternight.  Tries to talk Rand al'Thor to come with him to see the Myrddraal.  Rand kills him.  Eight feet tall, with a wolf's muzzle and goat hooves.</t>
+  </si>
+  <si>
+    <t>Kari al'Thor</t>
+  </si>
+  <si>
+    <t>Laman</t>
+  </si>
+  <si>
+    <t>Deceased mother of Rand.  Died when Rand was five years old.  Wife to Tam al'Thor.  Tam's delirious ravings tell Rand that Kari al'Thor was not his real mother.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rand carries him back to Emond's Field. In his delirium, he rants about the Aiel War and about finding Rand. </t>
+  </si>
+  <si>
+    <t>Tam gives him his sword. Trollocs attack the house. Tam is wounded. He kills the Trolloc, Narg.</t>
+  </si>
+  <si>
+    <t>He carries Tam back to Emond's Field, sees the black-cloaked rider again, and learns from Tam's ranting that he was adopted.</t>
+  </si>
+  <si>
+    <t>In his delirium, Tam al'Thor rants about Laman's sin - cutting down Avendoraldera.</t>
+  </si>
+  <si>
+    <t>Rand has heard stories that Avendesora belongs to the Green Man.</t>
+  </si>
+  <si>
+    <t>Green Man</t>
+  </si>
+  <si>
+    <t>Berin Thane</t>
+  </si>
+  <si>
+    <t>Abell Cauthon</t>
+  </si>
+  <si>
+    <t>Darl Coplin</t>
   </si>
 </sst>
 </file>
@@ -760,8 +1269,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1331,11 +1846,135 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A165" sqref="A165"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4934,4 +5573,1513 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="127.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>258</v>
+      </c>
+      <c r="B28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>258</v>
+      </c>
+      <c r="B30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>340</v>
+      </c>
+      <c r="B34" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>341</v>
+      </c>
+      <c r="B35" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>341</v>
+      </c>
+      <c r="B36" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>341</v>
+      </c>
+      <c r="B37" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>